<commit_message>
added util to check json files
</commit_message>
<xml_diff>
--- a/records/xlsx/thermal.xlsx
+++ b/records/xlsx/thermal.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I138"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1698,29 +1698,29 @@
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>14_1</t>
+          <t>2 meters</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr">
         <is>
-          <t>2 meters</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E39" s="1" t="inlineStr">
         <is>
-          <t>14_relaxed_blanked_2me-12222022162724.avi</t>
+          <t>14_holdbreathing_blanked_2me-12222022162951.avi</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>2255</v>
+        <v>1930</v>
       </c>
       <c r="G39" t="n">
-        <v>225.5</v>
+        <v>193</v>
       </c>
       <c r="H39" t="n">
         <v>10</v>
@@ -1735,17 +1735,21 @@
       <c r="A40" s="1" t="n"/>
       <c r="B40" s="1" t="n"/>
       <c r="C40" s="1" t="n"/>
-      <c r="D40" s="1" t="n"/>
+      <c r="D40" s="1" t="inlineStr">
+        <is>
+          <t>WOB</t>
+        </is>
+      </c>
       <c r="E40" s="1" t="inlineStr">
         <is>
-          <t>14_relaxed_wob_2me-12222022162257.avi</t>
+          <t>14_holdbreathing2_wob_2me-12222022162548.avi</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>2310</v>
+        <v>205</v>
       </c>
       <c r="G40" t="n">
-        <v>231</v>
+        <v>20.5</v>
       </c>
       <c r="H40" t="n">
         <v>10</v>
@@ -1758,60 +1762,60 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n"/>
-      <c r="B41" s="1" t="inlineStr">
+      <c r="B41" s="1" t="n"/>
+      <c r="C41" s="1" t="n"/>
+      <c r="D41" s="1" t="n"/>
+      <c r="E41" s="1" t="inlineStr">
+        <is>
+          <t>14_holdbreathing_wob_2me-12222022162453.avi</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>1296</v>
+      </c>
+      <c r="G41" t="n">
+        <v>129.6</v>
+      </c>
+      <c r="H41" t="n">
+        <v>10</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
         <is>
           <t>2 meters</t>
         </is>
       </c>
-      <c r="C41" s="1" t="inlineStr">
+      <c r="C42" s="1" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="D41" s="1" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="E41" s="1" t="inlineStr">
-        <is>
-          <t>14_holdbreathing_blanked_2me-12222022162951.avi</t>
-        </is>
-      </c>
-      <c r="F41" t="n">
-        <v>1930</v>
-      </c>
-      <c r="G41" t="n">
-        <v>193</v>
-      </c>
-      <c r="H41" t="n">
-        <v>10</v>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n"/>
-      <c r="B42" s="1" t="n"/>
-      <c r="C42" s="1" t="n"/>
       <c r="D42" s="1" t="inlineStr">
         <is>
-          <t>WOB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E42" s="1" t="inlineStr">
         <is>
-          <t>14_holdbreathing2_wob_2me-12222022162548.avi</t>
+          <t>15_holdingbreath_blanket_2me-12232022092537.avi</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>205</v>
+        <v>127</v>
       </c>
       <c r="G42" t="n">
-        <v>20.5</v>
+        <v>12.7</v>
       </c>
       <c r="H42" t="n">
         <v>10</v>
@@ -1829,14 +1833,14 @@
       <c r="D43" s="1" t="n"/>
       <c r="E43" s="1" t="inlineStr">
         <is>
-          <t>14_holdbreathing_wob_2me-12222022162453.avi</t>
+          <t>15_holdingbreath_blanket_2me-12232022092548.avi</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>1296</v>
+        <v>160</v>
       </c>
       <c r="G43" t="n">
-        <v>129.6</v>
+        <v>16</v>
       </c>
       <c r="H43" t="n">
         <v>10</v>
@@ -1848,36 +1852,20 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="B44" s="1" t="inlineStr">
-        <is>
-          <t>2 meters</t>
-        </is>
-      </c>
-      <c r="C44" s="1" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
-      <c r="D44" s="1" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+      <c r="A44" s="1" t="n"/>
+      <c r="B44" s="1" t="n"/>
+      <c r="C44" s="1" t="n"/>
+      <c r="D44" s="1" t="n"/>
       <c r="E44" s="1" t="inlineStr">
         <is>
-          <t>15_holdingbreath_blanket_2me-12232022092537.avi</t>
+          <t>15_holdingbreath_blanket_2me-12232022092600.avi</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>127</v>
+        <v>1</v>
       </c>
       <c r="G44" t="n">
-        <v>12.7</v>
+        <v>0.1</v>
       </c>
       <c r="H44" t="n">
         <v>10</v>
@@ -1895,14 +1883,14 @@
       <c r="D45" s="1" t="n"/>
       <c r="E45" s="1" t="inlineStr">
         <is>
-          <t>15_holdingbreath_blanket_2me-12232022092548.avi</t>
+          <t>15_holdingbreath_blanket_2me-12232022092720-0000.avi</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>160</v>
+        <v>29</v>
       </c>
       <c r="G45" t="n">
-        <v>16</v>
+        <v>2.9</v>
       </c>
       <c r="H45" t="n">
         <v>10</v>
@@ -1920,14 +1908,14 @@
       <c r="D46" s="1" t="n"/>
       <c r="E46" s="1" t="inlineStr">
         <is>
-          <t>15_holdingbreath_blanket_2me-12232022092600.avi</t>
+          <t>15_holdingbreath_blanket_2me-12232022092843-0000.avi</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="G46" t="n">
-        <v>0.1</v>
+        <v>2.5</v>
       </c>
       <c r="H46" t="n">
         <v>10</v>
@@ -1945,14 +1933,14 @@
       <c r="D47" s="1" t="n"/>
       <c r="E47" s="1" t="inlineStr">
         <is>
-          <t>15_holdingbreath_blanket_2me-12232022092720-0000.avi</t>
+          <t>15_holdingbreath_blanket_2me-12232022092857-0000.avi</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="G47" t="n">
-        <v>2.9</v>
+        <v>5</v>
       </c>
       <c r="H47" t="n">
         <v>10</v>
@@ -1970,14 +1958,14 @@
       <c r="D48" s="1" t="n"/>
       <c r="E48" s="1" t="inlineStr">
         <is>
-          <t>15_holdingbreath_blanket_2me-12232022092843-0000.avi</t>
+          <t>15_holdingbreath_blanket_2me-12232022092924-0000.avi</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G48" t="n">
-        <v>2.5</v>
+        <v>3.2</v>
       </c>
       <c r="H48" t="n">
         <v>10</v>
@@ -1992,17 +1980,21 @@
       <c r="A49" s="1" t="n"/>
       <c r="B49" s="1" t="n"/>
       <c r="C49" s="1" t="n"/>
-      <c r="D49" s="1" t="n"/>
+      <c r="D49" s="1" t="inlineStr">
+        <is>
+          <t>WOB</t>
+        </is>
+      </c>
       <c r="E49" s="1" t="inlineStr">
         <is>
-          <t>15_holdingbreath_blanket_2me-12232022092857-0000.avi</t>
+          <t>15_holdbreath_wob_2meters-12232022090750.avi</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="G49" t="n">
-        <v>5</v>
+        <v>11.4</v>
       </c>
       <c r="H49" t="n">
         <v>10</v>
@@ -2020,17 +2012,17 @@
       <c r="D50" s="1" t="n"/>
       <c r="E50" s="1" t="inlineStr">
         <is>
-          <t>15_holdingbreath_blanket_2me-12232022092924-0000.avi</t>
+          <t>15_holdbreath_wob_2meters-12232022090832.avi</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G50" t="n">
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
       <c r="H50" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
@@ -2042,24 +2034,20 @@
       <c r="A51" s="1" t="n"/>
       <c r="B51" s="1" t="n"/>
       <c r="C51" s="1" t="n"/>
-      <c r="D51" s="1" t="inlineStr">
-        <is>
-          <t>WOB</t>
-        </is>
-      </c>
+      <c r="D51" s="1" t="n"/>
       <c r="E51" s="1" t="inlineStr">
         <is>
-          <t>15_holdbreath_wob_2meters-12232022090750.avi</t>
+          <t>15_holdbreath_wob_2meters-12232022090914.avi</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>114</v>
+        <v>1</v>
       </c>
       <c r="G51" t="n">
-        <v>11.4</v>
+        <v>0.2</v>
       </c>
       <c r="H51" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
@@ -2074,17 +2062,17 @@
       <c r="D52" s="1" t="n"/>
       <c r="E52" s="1" t="inlineStr">
         <is>
-          <t>15_holdbreath_wob_2meters-12232022090832.avi</t>
+          <t>15_test_wob_2meters-12232022090012.avi</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="G52" t="n">
-        <v>2.8</v>
+        <v>6.4</v>
       </c>
       <c r="H52" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
@@ -2099,17 +2087,17 @@
       <c r="D53" s="1" t="n"/>
       <c r="E53" s="1" t="inlineStr">
         <is>
-          <t>15_holdbreath_wob_2meters-12232022090914.avi</t>
+          <t>15_test_wob_2meters-12232022090456.avi</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>1</v>
+        <v>176</v>
       </c>
       <c r="G53" t="n">
-        <v>0.2</v>
+        <v>17.6</v>
       </c>
       <c r="H53" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
@@ -2120,18 +2108,26 @@
     <row r="54">
       <c r="A54" s="1" t="n"/>
       <c r="B54" s="1" t="n"/>
-      <c r="C54" s="1" t="n"/>
-      <c r="D54" s="1" t="n"/>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D54" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
       <c r="E54" s="1" t="inlineStr">
         <is>
-          <t>15_test_wob_2meters-12232022090012.avi</t>
+          <t>15_relaxed_blanket_2me-12232022091943.avi</t>
         </is>
       </c>
       <c r="F54" t="n">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="G54" t="n">
-        <v>6.4</v>
+        <v>2.7</v>
       </c>
       <c r="H54" t="n">
         <v>10</v>
@@ -2149,14 +2145,14 @@
       <c r="D55" s="1" t="n"/>
       <c r="E55" s="1" t="inlineStr">
         <is>
-          <t>15_test_wob_2meters-12232022090456.avi</t>
+          <t>15_relaxed_blanket_2me-12232022092035.avi</t>
         </is>
       </c>
       <c r="F55" t="n">
-        <v>176</v>
+        <v>66</v>
       </c>
       <c r="G55" t="n">
-        <v>17.6</v>
+        <v>6.6</v>
       </c>
       <c r="H55" t="n">
         <v>10</v>
@@ -2170,26 +2166,18 @@
     <row r="56">
       <c r="A56" s="1" t="n"/>
       <c r="B56" s="1" t="n"/>
-      <c r="C56" s="1" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="D56" s="1" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+      <c r="C56" s="1" t="n"/>
+      <c r="D56" s="1" t="n"/>
       <c r="E56" s="1" t="inlineStr">
         <is>
-          <t>15_relaxed_blanket_2me-12232022091943.avi</t>
+          <t>15_relaxed_blanket_2me-12232022092305.avi</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>27</v>
+        <v>543</v>
       </c>
       <c r="G56" t="n">
-        <v>2.7</v>
+        <v>54.3</v>
       </c>
       <c r="H56" t="n">
         <v>10</v>
@@ -2207,14 +2195,14 @@
       <c r="D57" s="1" t="n"/>
       <c r="E57" s="1" t="inlineStr">
         <is>
-          <t>15_relaxed_blanket_2me-12232022092035.avi</t>
+          <t>15_relaxed_blanket_2me-12232022092332.avi</t>
         </is>
       </c>
       <c r="F57" t="n">
-        <v>66</v>
+        <v>633</v>
       </c>
       <c r="G57" t="n">
-        <v>6.6</v>
+        <v>63.3</v>
       </c>
       <c r="H57" t="n">
         <v>10</v>
@@ -2229,17 +2217,21 @@
       <c r="A58" s="1" t="n"/>
       <c r="B58" s="1" t="n"/>
       <c r="C58" s="1" t="n"/>
-      <c r="D58" s="1" t="n"/>
+      <c r="D58" s="1" t="inlineStr">
+        <is>
+          <t>WOB</t>
+        </is>
+      </c>
       <c r="E58" s="1" t="inlineStr">
         <is>
-          <t>15_relaxed_blanket_2me-12232022092305.avi</t>
+          <t>15_relaxed_wob_2meters-12232022085117.avi</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>543</v>
+        <v>995</v>
       </c>
       <c r="G58" t="n">
-        <v>54.3</v>
+        <v>99.5</v>
       </c>
       <c r="H58" t="n">
         <v>10</v>
@@ -2257,14 +2249,14 @@
       <c r="D59" s="1" t="n"/>
       <c r="E59" s="1" t="inlineStr">
         <is>
-          <t>15_relaxed_blanket_2me-12232022092332.avi</t>
+          <t>15_relaxed_wob_2meters-12232022085205.avi</t>
         </is>
       </c>
       <c r="F59" t="n">
-        <v>633</v>
+        <v>1</v>
       </c>
       <c r="G59" t="n">
-        <v>63.3</v>
+        <v>0.1</v>
       </c>
       <c r="H59" t="n">
         <v>10</v>
@@ -2279,21 +2271,17 @@
       <c r="A60" s="1" t="n"/>
       <c r="B60" s="1" t="n"/>
       <c r="C60" s="1" t="n"/>
-      <c r="D60" s="1" t="inlineStr">
-        <is>
-          <t>WOB</t>
-        </is>
-      </c>
+      <c r="D60" s="1" t="n"/>
       <c r="E60" s="1" t="inlineStr">
         <is>
-          <t>15_relaxed_wob_2meters-12232022085117.avi</t>
+          <t>15_relaxed_wob_2meters-12232022085212.avi</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>995</v>
+        <v>105</v>
       </c>
       <c r="G60" t="n">
-        <v>99.5</v>
+        <v>10.5</v>
       </c>
       <c r="H60" t="n">
         <v>10</v>
@@ -2311,14 +2299,14 @@
       <c r="D61" s="1" t="n"/>
       <c r="E61" s="1" t="inlineStr">
         <is>
-          <t>15_relaxed_wob_2meters-12232022085205.avi</t>
+          <t>15_relaxed_wob_2meters-12232022085224.avi</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="G61" t="n">
-        <v>0.1</v>
+        <v>5.6</v>
       </c>
       <c r="H61" t="n">
         <v>10</v>
@@ -2336,14 +2324,14 @@
       <c r="D62" s="1" t="n"/>
       <c r="E62" s="1" t="inlineStr">
         <is>
-          <t>15_relaxed_wob_2meters-12232022085212.avi</t>
+          <t>15_relaxed_wob_2meters-12232022085242.avi</t>
         </is>
       </c>
       <c r="F62" t="n">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="G62" t="n">
-        <v>10.5</v>
+        <v>20.6</v>
       </c>
       <c r="H62" t="n">
         <v>10</v>
@@ -2361,17 +2349,17 @@
       <c r="D63" s="1" t="n"/>
       <c r="E63" s="1" t="inlineStr">
         <is>
-          <t>15_relaxed_wob_2meters-12232022085224.avi</t>
+          <t>15_relaxed_wob_2meters-12232022085306.avi</t>
         </is>
       </c>
       <c r="F63" t="n">
-        <v>56</v>
+        <v>391</v>
       </c>
       <c r="G63" t="n">
-        <v>5.6</v>
+        <v>78.2</v>
       </c>
       <c r="H63" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I63" t="inlineStr">
         <is>
@@ -2386,17 +2374,17 @@
       <c r="D64" s="1" t="n"/>
       <c r="E64" s="1" t="inlineStr">
         <is>
-          <t>15_relaxed_wob_2meters-12232022085242.avi</t>
+          <t>15_relaxed_wob_2meters-12232022085332.avi</t>
         </is>
       </c>
       <c r="F64" t="n">
-        <v>206</v>
+        <v>28</v>
       </c>
       <c r="G64" t="n">
-        <v>20.6</v>
+        <v>5.6</v>
       </c>
       <c r="H64" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I64" t="inlineStr">
         <is>
@@ -2411,14 +2399,14 @@
       <c r="D65" s="1" t="n"/>
       <c r="E65" s="1" t="inlineStr">
         <is>
-          <t>15_relaxed_wob_2meters-12232022085306.avi</t>
+          <t>15_relaxed_wob_2meters-12232022085344.avi</t>
         </is>
       </c>
       <c r="F65" t="n">
-        <v>391</v>
+        <v>77</v>
       </c>
       <c r="G65" t="n">
-        <v>78.2</v>
+        <v>15.4</v>
       </c>
       <c r="H65" t="n">
         <v>5</v>
@@ -2436,14 +2424,14 @@
       <c r="D66" s="1" t="n"/>
       <c r="E66" s="1" t="inlineStr">
         <is>
-          <t>15_relaxed_wob_2meters-12232022085332.avi</t>
+          <t>15_relaxed_wob_2meters-12232022085400.avi</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="G66" t="n">
-        <v>5.6</v>
+        <v>18.4</v>
       </c>
       <c r="H66" t="n">
         <v>5</v>
@@ -2455,23 +2443,39 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="n"/>
-      <c r="B67" s="1" t="n"/>
-      <c r="C67" s="1" t="n"/>
-      <c r="D67" s="1" t="n"/>
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B67" s="1" t="inlineStr">
+        <is>
+          <t>2 meters</t>
+        </is>
+      </c>
+      <c r="C67" s="1" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D67" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
       <c r="E67" s="1" t="inlineStr">
         <is>
-          <t>15_relaxed_wob_2meters-12232022085344.avi</t>
+          <t>2_H_B_2m-12222022100256.avi</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>77</v>
+        <v>4567</v>
       </c>
       <c r="G67" t="n">
-        <v>15.4</v>
+        <v>152.2333333333333</v>
       </c>
       <c r="H67" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="I67" t="inlineStr">
         <is>
@@ -2483,20 +2487,24 @@
       <c r="A68" s="1" t="n"/>
       <c r="B68" s="1" t="n"/>
       <c r="C68" s="1" t="n"/>
-      <c r="D68" s="1" t="n"/>
+      <c r="D68" s="1" t="inlineStr">
+        <is>
+          <t>WOB</t>
+        </is>
+      </c>
       <c r="E68" s="1" t="inlineStr">
         <is>
-          <t>15_relaxed_wob_2meters-12232022085400.avi</t>
+          <t>2_H_WOB_2m-12222022095411.avi</t>
         </is>
       </c>
       <c r="F68" t="n">
-        <v>92</v>
+        <v>4466</v>
       </c>
       <c r="G68" t="n">
-        <v>18.4</v>
+        <v>148.8666666666667</v>
       </c>
       <c r="H68" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="I68" t="inlineStr">
         <is>
@@ -2505,19 +2513,11 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B69" s="1" t="inlineStr">
-        <is>
-          <t>2 meters</t>
-        </is>
-      </c>
+      <c r="A69" s="1" t="n"/>
+      <c r="B69" s="1" t="n"/>
       <c r="C69" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>R</t>
         </is>
       </c>
       <c r="D69" s="1" t="inlineStr">
@@ -2527,14 +2527,14 @@
       </c>
       <c r="E69" s="1" t="inlineStr">
         <is>
-          <t>2_H_B_2m-12222022100256.avi</t>
+          <t>2_R_B_2m-12222022095917.avi</t>
         </is>
       </c>
       <c r="F69" t="n">
-        <v>4567</v>
+        <v>4691</v>
       </c>
       <c r="G69" t="n">
-        <v>152.2333333333333</v>
+        <v>156.3666666666667</v>
       </c>
       <c r="H69" t="n">
         <v>30</v>
@@ -2556,14 +2556,14 @@
       </c>
       <c r="E70" s="1" t="inlineStr">
         <is>
-          <t>2_H_WOB_2m-12222022095411.avi</t>
+          <t>2_R_WOB_2m-12222022095034.avi</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>4466</v>
+        <v>4344</v>
       </c>
       <c r="G70" t="n">
-        <v>148.8666666666667</v>
+        <v>144.8</v>
       </c>
       <c r="H70" t="n">
         <v>30</v>
@@ -2576,10 +2576,14 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n"/>
-      <c r="B71" s="1" t="n"/>
+      <c r="B71" s="1" t="inlineStr">
+        <is>
+          <t>3 meters</t>
+        </is>
+      </c>
       <c r="C71" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D71" s="1" t="inlineStr">
@@ -2589,14 +2593,14 @@
       </c>
       <c r="E71" s="1" t="inlineStr">
         <is>
-          <t>2_R_B_2m-12222022095917.avi</t>
+          <t>2_H_B_3m-12222022102602.avi</t>
         </is>
       </c>
       <c r="F71" t="n">
-        <v>4691</v>
+        <v>3992</v>
       </c>
       <c r="G71" t="n">
-        <v>156.3666666666667</v>
+        <v>133.0666666666667</v>
       </c>
       <c r="H71" t="n">
         <v>30</v>
@@ -2618,14 +2622,14 @@
       </c>
       <c r="E72" s="1" t="inlineStr">
         <is>
-          <t>2_R_WOB_2m-12222022095034.avi</t>
+          <t>2_H_WOB_3m-12222022101944.avi</t>
         </is>
       </c>
       <c r="F72" t="n">
-        <v>4344</v>
+        <v>3952</v>
       </c>
       <c r="G72" t="n">
-        <v>144.8</v>
+        <v>131.7333333333333</v>
       </c>
       <c r="H72" t="n">
         <v>30</v>
@@ -2638,14 +2642,10 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n"/>
-      <c r="B73" s="1" t="inlineStr">
-        <is>
-          <t>3 meters</t>
-        </is>
-      </c>
+      <c r="B73" s="1" t="n"/>
       <c r="C73" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>R</t>
         </is>
       </c>
       <c r="D73" s="1" t="inlineStr">
@@ -2655,14 +2655,14 @@
       </c>
       <c r="E73" s="1" t="inlineStr">
         <is>
-          <t>2_H_B_3m-12222022102602.avi</t>
+          <t>2_R_B_3m-12222022102314.avi</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>3992</v>
+        <v>3834</v>
       </c>
       <c r="G73" t="n">
-        <v>133.0666666666667</v>
+        <v>127.8</v>
       </c>
       <c r="H73" t="n">
         <v>30</v>
@@ -2684,14 +2684,14 @@
       </c>
       <c r="E74" s="1" t="inlineStr">
         <is>
-          <t>2_H_WOB_3m-12222022101944.avi</t>
+          <t>2_R_WOB_3m-12222022101525.avi</t>
         </is>
       </c>
       <c r="F74" t="n">
-        <v>3952</v>
+        <v>656</v>
       </c>
       <c r="G74" t="n">
-        <v>131.7333333333333</v>
+        <v>21.86666666666667</v>
       </c>
       <c r="H74" t="n">
         <v>30</v>
@@ -2705,26 +2705,18 @@
     <row r="75">
       <c r="A75" s="1" t="n"/>
       <c r="B75" s="1" t="n"/>
-      <c r="C75" s="1" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="D75" s="1" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+      <c r="C75" s="1" t="n"/>
+      <c r="D75" s="1" t="n"/>
       <c r="E75" s="1" t="inlineStr">
         <is>
-          <t>2_R_B_3m-12222022102314.avi</t>
+          <t>2_R_WOB_3m-12222022101644.avi</t>
         </is>
       </c>
       <c r="F75" t="n">
-        <v>3834</v>
+        <v>3880</v>
       </c>
       <c r="G75" t="n">
-        <v>127.8</v>
+        <v>129.3333333333333</v>
       </c>
       <c r="H75" t="n">
         <v>30</v>
@@ -2736,24 +2728,36 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="n"/>
-      <c r="B76" s="1" t="n"/>
-      <c r="C76" s="1" t="n"/>
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B76" s="1" t="inlineStr">
+        <is>
+          <t>3 meters</t>
+        </is>
+      </c>
+      <c r="C76" s="1" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
       <c r="D76" s="1" t="inlineStr">
         <is>
-          <t>WOB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E76" s="1" t="inlineStr">
         <is>
-          <t>2_R_WOB_3m-12222022101525.avi</t>
+          <t>3_HB_B_3m-12222022103839.avi</t>
         </is>
       </c>
       <c r="F76" t="n">
-        <v>656</v>
+        <v>3295</v>
       </c>
       <c r="G76" t="n">
-        <v>21.86666666666667</v>
+        <v>109.8333333333333</v>
       </c>
       <c r="H76" t="n">
         <v>30</v>
@@ -2768,17 +2772,21 @@
       <c r="A77" s="1" t="n"/>
       <c r="B77" s="1" t="n"/>
       <c r="C77" s="1" t="n"/>
-      <c r="D77" s="1" t="n"/>
+      <c r="D77" s="1" t="inlineStr">
+        <is>
+          <t>WOB</t>
+        </is>
+      </c>
       <c r="E77" s="1" t="inlineStr">
         <is>
-          <t>2_R_WOB_3m-12222022101644.avi</t>
+          <t>3_HB_WOB_3METERS-12222022104233.avi</t>
         </is>
       </c>
       <c r="F77" t="n">
-        <v>3880</v>
+        <v>3921</v>
       </c>
       <c r="G77" t="n">
-        <v>129.3333333333333</v>
+        <v>130.7</v>
       </c>
       <c r="H77" t="n">
         <v>30</v>
@@ -2790,19 +2798,11 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B78" s="1" t="inlineStr">
-        <is>
-          <t>3 meters</t>
-        </is>
-      </c>
+      <c r="A78" s="1" t="n"/>
+      <c r="B78" s="1" t="n"/>
       <c r="C78" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>R</t>
         </is>
       </c>
       <c r="D78" s="1" t="inlineStr">
@@ -2812,14 +2812,14 @@
       </c>
       <c r="E78" s="1" t="inlineStr">
         <is>
-          <t>3_HB_B_3m-12222022103839.avi</t>
+          <t>3_R_B_3METERS-12222022103546.avi</t>
         </is>
       </c>
       <c r="F78" t="n">
-        <v>3295</v>
+        <v>4064</v>
       </c>
       <c r="G78" t="n">
-        <v>109.8333333333333</v>
+        <v>135.4666666666667</v>
       </c>
       <c r="H78" t="n">
         <v>30</v>
@@ -2841,14 +2841,14 @@
       </c>
       <c r="E79" s="1" t="inlineStr">
         <is>
-          <t>3_HB_WOB_3METERS-12222022104233.avi</t>
+          <t>3_R_WOB_3m-12222022103229.avi</t>
         </is>
       </c>
       <c r="F79" t="n">
-        <v>3921</v>
+        <v>3949</v>
       </c>
       <c r="G79" t="n">
-        <v>130.7</v>
+        <v>131.6333333333333</v>
       </c>
       <c r="H79" t="n">
         <v>30</v>
@@ -2860,11 +2860,19 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="n"/>
-      <c r="B80" s="1" t="n"/>
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B80" s="1" t="inlineStr">
+        <is>
+          <t>2 meters</t>
+        </is>
+      </c>
       <c r="C80" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D80" s="1" t="inlineStr">
@@ -2874,14 +2882,14 @@
       </c>
       <c r="E80" s="1" t="inlineStr">
         <is>
-          <t>3_R_B_3METERS-12222022103546.avi</t>
+          <t>4_b_holdbreath_2METERS-12222022113635.avi</t>
         </is>
       </c>
       <c r="F80" t="n">
-        <v>4064</v>
+        <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>135.4666666666667</v>
+        <v>0</v>
       </c>
       <c r="H80" t="n">
         <v>30</v>
@@ -2896,21 +2904,17 @@
       <c r="A81" s="1" t="n"/>
       <c r="B81" s="1" t="n"/>
       <c r="C81" s="1" t="n"/>
-      <c r="D81" s="1" t="inlineStr">
-        <is>
-          <t>WOB</t>
-        </is>
-      </c>
+      <c r="D81" s="1" t="n"/>
       <c r="E81" s="1" t="inlineStr">
         <is>
-          <t>3_R_WOB_3m-12222022103229.avi</t>
+          <t>4_b_holdbreath_2METERS-12222022113645.avi</t>
         </is>
       </c>
       <c r="F81" t="n">
-        <v>3949</v>
+        <v>4756</v>
       </c>
       <c r="G81" t="n">
-        <v>131.6333333333333</v>
+        <v>158.5333333333333</v>
       </c>
       <c r="H81" t="n">
         <v>30</v>
@@ -2922,36 +2926,24 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B82" s="1" t="inlineStr">
-        <is>
-          <t>2 meters</t>
-        </is>
-      </c>
-      <c r="C82" s="1" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
+      <c r="A82" s="1" t="n"/>
+      <c r="B82" s="1" t="n"/>
+      <c r="C82" s="1" t="n"/>
       <c r="D82" s="1" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>WOB</t>
         </is>
       </c>
       <c r="E82" s="1" t="inlineStr">
         <is>
-          <t>4_b_holdbreath_2METERS-12222022113635.avi</t>
+          <t>4_wob_HoldBreath_2METERS-12222022112005-12222022112746.avi</t>
         </is>
       </c>
       <c r="F82" t="n">
-        <v>0</v>
+        <v>2626</v>
       </c>
       <c r="G82" t="n">
-        <v>0</v>
+        <v>87.53333333333333</v>
       </c>
       <c r="H82" t="n">
         <v>30</v>
@@ -2965,18 +2957,26 @@
     <row r="83">
       <c r="A83" s="1" t="n"/>
       <c r="B83" s="1" t="n"/>
-      <c r="C83" s="1" t="n"/>
-      <c r="D83" s="1" t="n"/>
+      <c r="C83" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D83" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
       <c r="E83" s="1" t="inlineStr">
         <is>
-          <t>4_b_holdbreath_2METERS-12222022113645.avi</t>
+          <t>4_b_relaxed_2METERS-12222022113126.avi</t>
         </is>
       </c>
       <c r="F83" t="n">
-        <v>4756</v>
+        <v>3821</v>
       </c>
       <c r="G83" t="n">
-        <v>158.5333333333333</v>
+        <v>127.3666666666667</v>
       </c>
       <c r="H83" t="n">
         <v>30</v>
@@ -2998,14 +2998,14 @@
       </c>
       <c r="E84" s="1" t="inlineStr">
         <is>
-          <t>4_wob_HoldBreath_2METERS-12222022112005-12222022112746.avi</t>
+          <t>4_wob_relaxed_2METERS-12222022112005-12222022112340.avi</t>
         </is>
       </c>
       <c r="F84" t="n">
-        <v>2626</v>
+        <v>4594</v>
       </c>
       <c r="G84" t="n">
-        <v>87.53333333333333</v>
+        <v>153.1333333333333</v>
       </c>
       <c r="H84" t="n">
         <v>30</v>
@@ -3018,10 +3018,14 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n"/>
-      <c r="B85" s="1" t="n"/>
+      <c r="B85" s="1" t="inlineStr">
+        <is>
+          <t>3 meters</t>
+        </is>
+      </c>
       <c r="C85" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D85" s="1" t="inlineStr">
@@ -3031,14 +3035,14 @@
       </c>
       <c r="E85" s="1" t="inlineStr">
         <is>
-          <t>4_b_relaxed_2METERS-12222022113126.avi</t>
+          <t>4_holdbreth_blanket_3ME-12222022115812.avi</t>
         </is>
       </c>
       <c r="F85" t="n">
-        <v>3821</v>
+        <v>4683</v>
       </c>
       <c r="G85" t="n">
-        <v>127.3666666666667</v>
+        <v>156.1</v>
       </c>
       <c r="H85" t="n">
         <v>30</v>
@@ -3060,14 +3064,14 @@
       </c>
       <c r="E86" s="1" t="inlineStr">
         <is>
-          <t>4_wob_relaxed_2METERS-12222022112005-12222022112340.avi</t>
+          <t>4_holdbreathing_wob_3ME-12222022115105.avi</t>
         </is>
       </c>
       <c r="F86" t="n">
-        <v>4594</v>
+        <v>3855</v>
       </c>
       <c r="G86" t="n">
-        <v>153.1333333333333</v>
+        <v>128.5</v>
       </c>
       <c r="H86" t="n">
         <v>30</v>
@@ -3080,14 +3084,10 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n"/>
-      <c r="B87" s="1" t="inlineStr">
-        <is>
-          <t>3 meters</t>
-        </is>
-      </c>
+      <c r="B87" s="1" t="n"/>
       <c r="C87" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>R</t>
         </is>
       </c>
       <c r="D87" s="1" t="inlineStr">
@@ -3097,14 +3097,14 @@
       </c>
       <c r="E87" s="1" t="inlineStr">
         <is>
-          <t>4_holdbreth_blanket_3ME-12222022115812.avi</t>
+          <t>4_relaxed_b_3ME-12222022115452.avi</t>
         </is>
       </c>
       <c r="F87" t="n">
-        <v>4683</v>
+        <v>3871</v>
       </c>
       <c r="G87" t="n">
-        <v>156.1</v>
+        <v>129.0333333333333</v>
       </c>
       <c r="H87" t="n">
         <v>30</v>
@@ -3126,17 +3126,17 @@
       </c>
       <c r="E88" s="1" t="inlineStr">
         <is>
-          <t>4_holdbreathing_wob_3ME-12222022115105.avi</t>
+          <t>4_relaxed_wob_3ME-12222022114801-0000.avi</t>
         </is>
       </c>
       <c r="F88" t="n">
-        <v>3855</v>
+        <v>124</v>
       </c>
       <c r="G88" t="n">
-        <v>128.5</v>
+        <v>4.133292</v>
       </c>
       <c r="H88" t="n">
-        <v>30</v>
+        <v>30.00030000300003</v>
       </c>
       <c r="I88" t="inlineStr">
         <is>
@@ -3147,26 +3147,18 @@
     <row r="89">
       <c r="A89" s="1" t="n"/>
       <c r="B89" s="1" t="n"/>
-      <c r="C89" s="1" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="D89" s="1" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+      <c r="C89" s="1" t="n"/>
+      <c r="D89" s="1" t="n"/>
       <c r="E89" s="1" t="inlineStr">
         <is>
-          <t>4_relaxed_b_3ME-12222022115452.avi</t>
+          <t>4_relaxed_wob_3ME-12222022114811.avi</t>
         </is>
       </c>
       <c r="F89" t="n">
-        <v>3871</v>
+        <v>3497</v>
       </c>
       <c r="G89" t="n">
-        <v>129.0333333333333</v>
+        <v>116.5666666666667</v>
       </c>
       <c r="H89" t="n">
         <v>30</v>
@@ -3178,27 +3170,39 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="1" t="n"/>
-      <c r="B90" s="1" t="n"/>
-      <c r="C90" s="1" t="n"/>
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B90" s="1" t="inlineStr">
+        <is>
+          <t>2 meters</t>
+        </is>
+      </c>
+      <c r="C90" s="1" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
       <c r="D90" s="1" t="inlineStr">
         <is>
-          <t>WOB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E90" s="1" t="inlineStr">
         <is>
-          <t>4_relaxed_wob_3ME-12222022114801-0000.avi</t>
+          <t>5_holdbreath_blanked_2me-12222022134041.avi</t>
         </is>
       </c>
       <c r="F90" t="n">
-        <v>124</v>
+        <v>3579</v>
       </c>
       <c r="G90" t="n">
-        <v>4.133292</v>
+        <v>357.9</v>
       </c>
       <c r="H90" t="n">
-        <v>30.00030000300003</v>
+        <v>10</v>
       </c>
       <c r="I90" t="inlineStr">
         <is>
@@ -3210,20 +3214,24 @@
       <c r="A91" s="1" t="n"/>
       <c r="B91" s="1" t="n"/>
       <c r="C91" s="1" t="n"/>
-      <c r="D91" s="1" t="n"/>
+      <c r="D91" s="1" t="inlineStr">
+        <is>
+          <t>WOB</t>
+        </is>
+      </c>
       <c r="E91" s="1" t="inlineStr">
         <is>
-          <t>4_relaxed_wob_3ME-12222022114811.avi</t>
+          <t>5_holdbreath_wob_2me-12222022133505.avi</t>
         </is>
       </c>
       <c r="F91" t="n">
-        <v>3497</v>
+        <v>3471</v>
       </c>
       <c r="G91" t="n">
-        <v>116.5666666666667</v>
+        <v>347.1</v>
       </c>
       <c r="H91" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I91" t="inlineStr">
         <is>
@@ -3232,19 +3240,11 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B92" s="1" t="inlineStr">
-        <is>
-          <t>2 meters</t>
-        </is>
-      </c>
+      <c r="A92" s="1" t="n"/>
+      <c r="B92" s="1" t="n"/>
       <c r="C92" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>R</t>
         </is>
       </c>
       <c r="D92" s="1" t="inlineStr">
@@ -3254,14 +3254,14 @@
       </c>
       <c r="E92" s="1" t="inlineStr">
         <is>
-          <t>5_holdbreath_blanked_2me-12222022134041.avi</t>
+          <t>5_relaxed_blamked_2me-12222022133744.avi</t>
         </is>
       </c>
       <c r="F92" t="n">
-        <v>3579</v>
+        <v>4450</v>
       </c>
       <c r="G92" t="n">
-        <v>357.9</v>
+        <v>445</v>
       </c>
       <c r="H92" t="n">
         <v>10</v>
@@ -3283,14 +3283,14 @@
       </c>
       <c r="E93" s="1" t="inlineStr">
         <is>
-          <t>5_holdbreath_wob_2me-12222022133505.avi</t>
+          <t>5_relaxed_wob_2me-12222022133228.avi</t>
         </is>
       </c>
       <c r="F93" t="n">
-        <v>3471</v>
+        <v>3554</v>
       </c>
       <c r="G93" t="n">
-        <v>347.1</v>
+        <v>355.4</v>
       </c>
       <c r="H93" t="n">
         <v>10</v>
@@ -3303,10 +3303,14 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n"/>
-      <c r="B94" s="1" t="n"/>
+      <c r="B94" s="1" t="inlineStr">
+        <is>
+          <t>3 meters</t>
+        </is>
+      </c>
       <c r="C94" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D94" s="1" t="inlineStr">
@@ -3316,17 +3320,17 @@
       </c>
       <c r="E94" s="1" t="inlineStr">
         <is>
-          <t>5_relaxed_blamked_2me-12222022133744.avi</t>
+          <t>5_holdbrething_blanket_3ME-12222022121630.avi</t>
         </is>
       </c>
       <c r="F94" t="n">
-        <v>4450</v>
+        <v>4079</v>
       </c>
       <c r="G94" t="n">
-        <v>445</v>
+        <v>135.9666666666667</v>
       </c>
       <c r="H94" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I94" t="inlineStr">
         <is>
@@ -3345,17 +3349,17 @@
       </c>
       <c r="E95" s="1" t="inlineStr">
         <is>
-          <t>5_relaxed_wob_2me-12222022133228.avi</t>
+          <t>5_holding_wob_3ME-12222022120954.avi</t>
         </is>
       </c>
       <c r="F95" t="n">
-        <v>3554</v>
+        <v>4041</v>
       </c>
       <c r="G95" t="n">
-        <v>355.4</v>
+        <v>134.7</v>
       </c>
       <c r="H95" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I95" t="inlineStr">
         <is>
@@ -3365,14 +3369,10 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n"/>
-      <c r="B96" s="1" t="inlineStr">
-        <is>
-          <t>3 meters</t>
-        </is>
-      </c>
+      <c r="B96" s="1" t="n"/>
       <c r="C96" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>R</t>
         </is>
       </c>
       <c r="D96" s="1" t="inlineStr">
@@ -3382,14 +3382,14 @@
       </c>
       <c r="E96" s="1" t="inlineStr">
         <is>
-          <t>5_holdbrething_blanket_3ME-12222022121630.avi</t>
+          <t>5_relax_blanket_3ME-12222022121330.avi</t>
         </is>
       </c>
       <c r="F96" t="n">
-        <v>4079</v>
+        <v>4026</v>
       </c>
       <c r="G96" t="n">
-        <v>135.9666666666667</v>
+        <v>134.2</v>
       </c>
       <c r="H96" t="n">
         <v>30</v>
@@ -3411,14 +3411,14 @@
       </c>
       <c r="E97" s="1" t="inlineStr">
         <is>
-          <t>5_holding_wob_3ME-12222022120954.avi</t>
+          <t>5_relaxed_wob_3ME-12222022120703.avi</t>
         </is>
       </c>
       <c r="F97" t="n">
-        <v>4041</v>
+        <v>3556</v>
       </c>
       <c r="G97" t="n">
-        <v>134.7</v>
+        <v>118.5333333333333</v>
       </c>
       <c r="H97" t="n">
         <v>30</v>
@@ -3430,11 +3430,19 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="n"/>
-      <c r="B98" s="1" t="n"/>
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B98" s="1" t="inlineStr">
+        <is>
+          <t>2 meters</t>
+        </is>
+      </c>
       <c r="C98" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D98" s="1" t="inlineStr">
@@ -3444,17 +3452,17 @@
       </c>
       <c r="E98" s="1" t="inlineStr">
         <is>
-          <t>5_relax_blanket_3ME-12222022121330.avi</t>
+          <t>6_holding_blanket_2me-12222022161854.avi</t>
         </is>
       </c>
       <c r="F98" t="n">
-        <v>4026</v>
+        <v>2186</v>
       </c>
       <c r="G98" t="n">
-        <v>134.2</v>
+        <v>218.6</v>
       </c>
       <c r="H98" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I98" t="inlineStr">
         <is>
@@ -3473,17 +3481,17 @@
       </c>
       <c r="E99" s="1" t="inlineStr">
         <is>
-          <t>5_relaxed_wob_3ME-12222022120703.avi</t>
+          <t>6_holdingbbreath_wob_2me-12222022161254.avi</t>
         </is>
       </c>
       <c r="F99" t="n">
-        <v>3556</v>
+        <v>2214</v>
       </c>
       <c r="G99" t="n">
-        <v>118.5333333333333</v>
+        <v>221.4</v>
       </c>
       <c r="H99" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I99" t="inlineStr">
         <is>
@@ -3492,19 +3500,11 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B100" s="1" t="inlineStr">
-        <is>
-          <t>2 meters</t>
-        </is>
-      </c>
+      <c r="A100" s="1" t="n"/>
+      <c r="B100" s="1" t="n"/>
       <c r="C100" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>R</t>
         </is>
       </c>
       <c r="D100" s="1" t="inlineStr">
@@ -3514,14 +3514,14 @@
       </c>
       <c r="E100" s="1" t="inlineStr">
         <is>
-          <t>6_holding_blanket_2me-12222022161854.avi</t>
+          <t>6_relax_blanket_2me-12222022161616.avi</t>
         </is>
       </c>
       <c r="F100" t="n">
-        <v>2186</v>
+        <v>2566</v>
       </c>
       <c r="G100" t="n">
-        <v>218.6</v>
+        <v>256.6</v>
       </c>
       <c r="H100" t="n">
         <v>10</v>
@@ -3543,14 +3543,14 @@
       </c>
       <c r="E101" s="1" t="inlineStr">
         <is>
-          <t>6_holdingbbreath_wob_2me-12222022161254.avi</t>
+          <t>6_relaxed_wob_2me-12222022161005.avi</t>
         </is>
       </c>
       <c r="F101" t="n">
-        <v>2214</v>
+        <v>2438</v>
       </c>
       <c r="G101" t="n">
-        <v>221.4</v>
+        <v>243.8</v>
       </c>
       <c r="H101" t="n">
         <v>10</v>
@@ -3563,10 +3563,14 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="n"/>
-      <c r="B102" s="1" t="n"/>
+      <c r="B102" s="1" t="inlineStr">
+        <is>
+          <t>3 meters</t>
+        </is>
+      </c>
       <c r="C102" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D102" s="1" t="inlineStr">
@@ -3576,14 +3580,14 @@
       </c>
       <c r="E102" s="1" t="inlineStr">
         <is>
-          <t>6_relax_blanket_2me-12222022161616.avi</t>
+          <t>6_holdbreath_blanketvairable2_3ME_-12222022125229.avi</t>
         </is>
       </c>
       <c r="F102" t="n">
-        <v>2566</v>
+        <v>4844</v>
       </c>
       <c r="G102" t="n">
-        <v>256.6</v>
+        <v>484.4</v>
       </c>
       <c r="H102" t="n">
         <v>10</v>
@@ -3598,21 +3602,17 @@
       <c r="A103" s="1" t="n"/>
       <c r="B103" s="1" t="n"/>
       <c r="C103" s="1" t="n"/>
-      <c r="D103" s="1" t="inlineStr">
-        <is>
-          <t>WOB</t>
-        </is>
-      </c>
+      <c r="D103" s="1" t="n"/>
       <c r="E103" s="1" t="inlineStr">
         <is>
-          <t>6_relaxed_wob_2me-12222022161005.avi</t>
+          <t>6_holdbreath_blanket_3ME-12222022124654.avi</t>
         </is>
       </c>
       <c r="F103" t="n">
-        <v>2438</v>
+        <v>1452</v>
       </c>
       <c r="G103" t="n">
-        <v>243.8</v>
+        <v>145.2</v>
       </c>
       <c r="H103" t="n">
         <v>10</v>
@@ -3625,31 +3625,19 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="n"/>
-      <c r="B104" s="1" t="inlineStr">
-        <is>
-          <t>3 meters</t>
-        </is>
-      </c>
-      <c r="C104" s="1" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
-      <c r="D104" s="1" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+      <c r="B104" s="1" t="n"/>
+      <c r="C104" s="1" t="n"/>
+      <c r="D104" s="1" t="n"/>
       <c r="E104" s="1" t="inlineStr">
         <is>
-          <t>6_holdbreath_blanketvairable2_3ME_-12222022125229.avi</t>
+          <t>6_holdbreath_blanket_3ME_x2-12222022124816.avi</t>
         </is>
       </c>
       <c r="F104" t="n">
-        <v>4844</v>
+        <v>3246</v>
       </c>
       <c r="G104" t="n">
-        <v>484.4</v>
+        <v>324.6</v>
       </c>
       <c r="H104" t="n">
         <v>10</v>
@@ -3664,20 +3652,24 @@
       <c r="A105" s="1" t="n"/>
       <c r="B105" s="1" t="n"/>
       <c r="C105" s="1" t="n"/>
-      <c r="D105" s="1" t="n"/>
+      <c r="D105" s="1" t="inlineStr">
+        <is>
+          <t>WOB</t>
+        </is>
+      </c>
       <c r="E105" s="1" t="inlineStr">
         <is>
-          <t>6_holdbreath_blanket_3ME-12222022124654.avi</t>
+          <t>6_heldbreath2_WOB_3ME-12222022123516.avi</t>
         </is>
       </c>
       <c r="F105" t="n">
-        <v>1452</v>
+        <v>2703</v>
       </c>
       <c r="G105" t="n">
-        <v>145.2</v>
+        <v>90.09999999999999</v>
       </c>
       <c r="H105" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I105" t="inlineStr">
         <is>
@@ -3692,17 +3684,17 @@
       <c r="D106" s="1" t="n"/>
       <c r="E106" s="1" t="inlineStr">
         <is>
-          <t>6_holdbreath_blanket_3ME_x2-12222022124816.avi</t>
+          <t>6_heldbreath_WOB_3ME-12222022122738.avi</t>
         </is>
       </c>
       <c r="F106" t="n">
-        <v>3246</v>
+        <v>1538</v>
       </c>
       <c r="G106" t="n">
-        <v>324.6</v>
+        <v>51.26666666666667</v>
       </c>
       <c r="H106" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I106" t="inlineStr">
         <is>
@@ -3714,21 +3706,17 @@
       <c r="A107" s="1" t="n"/>
       <c r="B107" s="1" t="n"/>
       <c r="C107" s="1" t="n"/>
-      <c r="D107" s="1" t="inlineStr">
-        <is>
-          <t>WOB</t>
-        </is>
-      </c>
+      <c r="D107" s="1" t="n"/>
       <c r="E107" s="1" t="inlineStr">
         <is>
-          <t>6_heldbreath2_WOB_3ME-12222022123516.avi</t>
+          <t>6_heldbreath_WOB_3ME-12222022122914.avi</t>
         </is>
       </c>
       <c r="F107" t="n">
-        <v>2703</v>
+        <v>1423</v>
       </c>
       <c r="G107" t="n">
-        <v>90.09999999999999</v>
+        <v>47.43333333333333</v>
       </c>
       <c r="H107" t="n">
         <v>30</v>
@@ -3742,21 +3730,29 @@
     <row r="108">
       <c r="A108" s="1" t="n"/>
       <c r="B108" s="1" t="n"/>
-      <c r="C108" s="1" t="n"/>
-      <c r="D108" s="1" t="n"/>
+      <c r="C108" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D108" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
       <c r="E108" s="1" t="inlineStr">
         <is>
-          <t>6_heldbreath_WOB_3ME-12222022122738.avi</t>
+          <t>6_relaxed_blanket_3ME-12222022124350.avi</t>
         </is>
       </c>
       <c r="F108" t="n">
-        <v>1538</v>
+        <v>3910</v>
       </c>
       <c r="G108" t="n">
-        <v>51.26666666666667</v>
+        <v>391</v>
       </c>
       <c r="H108" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I108" t="inlineStr">
         <is>
@@ -3768,17 +3764,21 @@
       <c r="A109" s="1" t="n"/>
       <c r="B109" s="1" t="n"/>
       <c r="C109" s="1" t="n"/>
-      <c r="D109" s="1" t="n"/>
+      <c r="D109" s="1" t="inlineStr">
+        <is>
+          <t>WOB</t>
+        </is>
+      </c>
       <c r="E109" s="1" t="inlineStr">
         <is>
-          <t>6_heldbreath_WOB_3ME-12222022122914.avi</t>
+          <t>6_relaxed_WOB_3ME-12222022122444.avi</t>
         </is>
       </c>
       <c r="F109" t="n">
-        <v>1423</v>
+        <v>3710</v>
       </c>
       <c r="G109" t="n">
-        <v>47.43333333333333</v>
+        <v>123.6666666666667</v>
       </c>
       <c r="H109" t="n">
         <v>30</v>
@@ -3790,11 +3790,19 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="n"/>
-      <c r="B110" s="1" t="n"/>
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B110" s="1" t="inlineStr">
+        <is>
+          <t>2 meters</t>
+        </is>
+      </c>
       <c r="C110" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D110" s="1" t="inlineStr">
@@ -3804,14 +3812,14 @@
       </c>
       <c r="E110" s="1" t="inlineStr">
         <is>
-          <t>6_relaxed_blanket_3ME-12222022124350.avi</t>
+          <t>7_holdbreathing_blankets_2me-12222022132801.avi</t>
         </is>
       </c>
       <c r="F110" t="n">
-        <v>3910</v>
+        <v>3585</v>
       </c>
       <c r="G110" t="n">
-        <v>391</v>
+        <v>358.5</v>
       </c>
       <c r="H110" t="n">
         <v>10</v>
@@ -3833,17 +3841,17 @@
       </c>
       <c r="E111" s="1" t="inlineStr">
         <is>
-          <t>6_relaxed_WOB_3ME-12222022122444.avi</t>
+          <t>7_holdbreath_wob_2me-12222022132145.avi</t>
         </is>
       </c>
       <c r="F111" t="n">
-        <v>3710</v>
+        <v>3453</v>
       </c>
       <c r="G111" t="n">
-        <v>123.6666666666667</v>
+        <v>345.3</v>
       </c>
       <c r="H111" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I111" t="inlineStr">
         <is>
@@ -3852,19 +3860,11 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B112" s="1" t="inlineStr">
-        <is>
-          <t>2 meters</t>
-        </is>
-      </c>
+      <c r="A112" s="1" t="n"/>
+      <c r="B112" s="1" t="n"/>
       <c r="C112" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>R</t>
         </is>
       </c>
       <c r="D112" s="1" t="inlineStr">
@@ -3874,14 +3874,14 @@
       </c>
       <c r="E112" s="1" t="inlineStr">
         <is>
-          <t>7_holdbreathing_blankets_2me-12222022132801.avi</t>
+          <t>7_relaxed_blankets_2me-12222022132436.avi</t>
         </is>
       </c>
       <c r="F112" t="n">
-        <v>3585</v>
+        <v>5048</v>
       </c>
       <c r="G112" t="n">
-        <v>358.5</v>
+        <v>504.8</v>
       </c>
       <c r="H112" t="n">
         <v>10</v>
@@ -3903,17 +3903,17 @@
       </c>
       <c r="E113" s="1" t="inlineStr">
         <is>
-          <t>7_holdbreath_wob_2me-12222022132145.avi</t>
+          <t>7_relax_wob_2me-12222022131934.avi</t>
         </is>
       </c>
       <c r="F113" t="n">
-        <v>3453</v>
+        <v>2593</v>
       </c>
       <c r="G113" t="n">
-        <v>345.3</v>
+        <v>86.43333333333334</v>
       </c>
       <c r="H113" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I113" t="inlineStr">
         <is>
@@ -3923,10 +3923,14 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n"/>
-      <c r="B114" s="1" t="n"/>
+      <c r="B114" s="1" t="inlineStr">
+        <is>
+          <t>3 meters</t>
+        </is>
+      </c>
       <c r="C114" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D114" s="1" t="inlineStr">
@@ -3936,14 +3940,14 @@
       </c>
       <c r="E114" s="1" t="inlineStr">
         <is>
-          <t>7_relaxed_blankets_2me-12222022132436.avi</t>
+          <t>7_holdbreathing_blanket_3ME_-12222022131008.avi</t>
         </is>
       </c>
       <c r="F114" t="n">
-        <v>5048</v>
+        <v>3611</v>
       </c>
       <c r="G114" t="n">
-        <v>504.8</v>
+        <v>361.1</v>
       </c>
       <c r="H114" t="n">
         <v>10</v>
@@ -3965,17 +3969,17 @@
       </c>
       <c r="E115" s="1" t="inlineStr">
         <is>
-          <t>7_relax_wob_2me-12222022131934.avi</t>
+          <t>7_holdbreathing_WOB_3ME_-12222022130357.avi</t>
         </is>
       </c>
       <c r="F115" t="n">
-        <v>2593</v>
+        <v>3599</v>
       </c>
       <c r="G115" t="n">
-        <v>86.43333333333334</v>
+        <v>359.9</v>
       </c>
       <c r="H115" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I115" t="inlineStr">
         <is>
@@ -3985,14 +3989,10 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="n"/>
-      <c r="B116" s="1" t="inlineStr">
-        <is>
-          <t>3 meters</t>
-        </is>
-      </c>
+      <c r="B116" s="1" t="n"/>
       <c r="C116" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>R</t>
         </is>
       </c>
       <c r="D116" s="1" t="inlineStr">
@@ -4002,14 +4002,14 @@
       </c>
       <c r="E116" s="1" t="inlineStr">
         <is>
-          <t>7_holdbreathing_blanket_3ME_-12222022131008.avi</t>
+          <t>7_relaxed_blanket_3ME_-12222022130717.avi</t>
         </is>
       </c>
       <c r="F116" t="n">
-        <v>3611</v>
+        <v>3946</v>
       </c>
       <c r="G116" t="n">
-        <v>361.1</v>
+        <v>394.6</v>
       </c>
       <c r="H116" t="n">
         <v>10</v>
@@ -4031,14 +4031,14 @@
       </c>
       <c r="E117" s="1" t="inlineStr">
         <is>
-          <t>7_holdbreathing_WOB_3ME_-12222022130357.avi</t>
+          <t>7_relax_WOB_3ME_-12222022130055.avi</t>
         </is>
       </c>
       <c r="F117" t="n">
-        <v>3599</v>
+        <v>3438</v>
       </c>
       <c r="G117" t="n">
-        <v>359.9</v>
+        <v>343.8</v>
       </c>
       <c r="H117" t="n">
         <v>10</v>
@@ -4050,11 +4050,19 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="n"/>
-      <c r="B118" s="1" t="n"/>
+      <c r="A118" s="1" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B118" s="1" t="inlineStr">
+        <is>
+          <t>2 meters</t>
+        </is>
+      </c>
       <c r="C118" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D118" s="1" t="inlineStr">
@@ -4064,14 +4072,14 @@
       </c>
       <c r="E118" s="1" t="inlineStr">
         <is>
-          <t>7_relaxed_blanket_3ME_-12222022130717.avi</t>
+          <t>8_holdbreathing_blanket_2me-12222022135956.avi</t>
         </is>
       </c>
       <c r="F118" t="n">
-        <v>3946</v>
+        <v>3544</v>
       </c>
       <c r="G118" t="n">
-        <v>394.6</v>
+        <v>354.4</v>
       </c>
       <c r="H118" t="n">
         <v>10</v>
@@ -4093,14 +4101,14 @@
       </c>
       <c r="E119" s="1" t="inlineStr">
         <is>
-          <t>7_relax_WOB_3ME_-12222022130055.avi</t>
+          <t>8_holdbreath_withoutblanked_2me-12222022135120.avi</t>
         </is>
       </c>
       <c r="F119" t="n">
-        <v>3438</v>
+        <v>3551</v>
       </c>
       <c r="G119" t="n">
-        <v>343.8</v>
+        <v>355.1</v>
       </c>
       <c r="H119" t="n">
         <v>10</v>
@@ -4112,36 +4120,20 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="1" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="B120" s="1" t="inlineStr">
-        <is>
-          <t>2 meters</t>
-        </is>
-      </c>
-      <c r="C120" s="1" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
-      <c r="D120" s="1" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
+      <c r="A120" s="1" t="n"/>
+      <c r="B120" s="1" t="n"/>
+      <c r="C120" s="1" t="n"/>
+      <c r="D120" s="1" t="n"/>
       <c r="E120" s="1" t="inlineStr">
         <is>
-          <t>8_holdbreathing_blanket_2me-12222022135956.avi</t>
+          <t>8_holdbreath_withoutblanked_2me-12222022135413.avi</t>
         </is>
       </c>
       <c r="F120" t="n">
-        <v>3544</v>
+        <v>3741</v>
       </c>
       <c r="G120" t="n">
-        <v>354.4</v>
+        <v>374.1</v>
       </c>
       <c r="H120" t="n">
         <v>10</v>
@@ -4155,22 +4147,26 @@
     <row r="121">
       <c r="A121" s="1" t="n"/>
       <c r="B121" s="1" t="n"/>
-      <c r="C121" s="1" t="n"/>
+      <c r="C121" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="D121" s="1" t="inlineStr">
         <is>
-          <t>WOB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E121" s="1" t="inlineStr">
         <is>
-          <t>8_holdbreath_withoutblanked_2me-12222022135120.avi</t>
+          <t>8_relaxed_blanked_2me-12222022134840.avi</t>
         </is>
       </c>
       <c r="F121" t="n">
-        <v>3551</v>
+        <v>3553</v>
       </c>
       <c r="G121" t="n">
-        <v>355.1</v>
+        <v>355.3</v>
       </c>
       <c r="H121" t="n">
         <v>10</v>
@@ -4188,14 +4184,14 @@
       <c r="D122" s="1" t="n"/>
       <c r="E122" s="1" t="inlineStr">
         <is>
-          <t>8_holdbreath_withoutblanked_2me-12222022135413.avi</t>
+          <t>8_relaxed_blanket_2me-12222022135727.avi</t>
         </is>
       </c>
       <c r="F122" t="n">
-        <v>3741</v>
+        <v>3550</v>
       </c>
       <c r="G122" t="n">
-        <v>374.1</v>
+        <v>355</v>
       </c>
       <c r="H122" t="n">
         <v>10</v>
@@ -4208,10 +4204,14 @@
     </row>
     <row r="123">
       <c r="A123" s="1" t="n"/>
-      <c r="B123" s="1" t="n"/>
+      <c r="B123" s="1" t="inlineStr">
+        <is>
+          <t>3 meters</t>
+        </is>
+      </c>
       <c r="C123" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D123" s="1" t="inlineStr">
@@ -4221,14 +4221,14 @@
       </c>
       <c r="E123" s="1" t="inlineStr">
         <is>
-          <t>8_relaxed_blanked_2me-12222022134840.avi</t>
+          <t>8_holdbreathin_blanked_3me-12222022142640.avi</t>
         </is>
       </c>
       <c r="F123" t="n">
-        <v>3553</v>
+        <v>1917</v>
       </c>
       <c r="G123" t="n">
-        <v>355.3</v>
+        <v>191.7</v>
       </c>
       <c r="H123" t="n">
         <v>10</v>
@@ -4243,17 +4243,21 @@
       <c r="A124" s="1" t="n"/>
       <c r="B124" s="1" t="n"/>
       <c r="C124" s="1" t="n"/>
-      <c r="D124" s="1" t="n"/>
+      <c r="D124" s="1" t="inlineStr">
+        <is>
+          <t>WOB</t>
+        </is>
+      </c>
       <c r="E124" s="1" t="inlineStr">
         <is>
-          <t>8_relaxed_blanket_2me-12222022135727.avi</t>
+          <t>8_holdbreathing_withoutblanked_3me-12222022142104.avi</t>
         </is>
       </c>
       <c r="F124" t="n">
-        <v>3550</v>
+        <v>3706</v>
       </c>
       <c r="G124" t="n">
-        <v>355</v>
+        <v>370.6</v>
       </c>
       <c r="H124" t="n">
         <v>10</v>
@@ -4266,14 +4270,10 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="n"/>
-      <c r="B125" s="1" t="inlineStr">
-        <is>
-          <t>3 meters</t>
-        </is>
-      </c>
+      <c r="B125" s="1" t="n"/>
       <c r="C125" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>R</t>
         </is>
       </c>
       <c r="D125" s="1" t="inlineStr">
@@ -4283,14 +4283,14 @@
       </c>
       <c r="E125" s="1" t="inlineStr">
         <is>
-          <t>8_holdbreathin_blanked_3me-12222022142640.avi</t>
+          <t>8_relaxed_blanked_3me-12222022142425.avi</t>
         </is>
       </c>
       <c r="F125" t="n">
-        <v>1917</v>
+        <v>1935</v>
       </c>
       <c r="G125" t="n">
-        <v>191.7</v>
+        <v>193.5</v>
       </c>
       <c r="H125" t="n">
         <v>10</v>
@@ -4312,14 +4312,14 @@
       </c>
       <c r="E126" s="1" t="inlineStr">
         <is>
-          <t>8_holdbreathing_withoutblanked_3me-12222022142104.avi</t>
+          <t>8_relaxed_withoutblanked_3me-12222022141804.avi</t>
         </is>
       </c>
       <c r="F126" t="n">
-        <v>3706</v>
+        <v>3569</v>
       </c>
       <c r="G126" t="n">
-        <v>370.6</v>
+        <v>356.9</v>
       </c>
       <c r="H126" t="n">
         <v>10</v>
@@ -4331,11 +4331,19 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="1" t="n"/>
-      <c r="B127" s="1" t="n"/>
+      <c r="A127" s="1" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B127" s="1" t="inlineStr">
+        <is>
+          <t>2 meters</t>
+        </is>
+      </c>
       <c r="C127" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D127" s="1" t="inlineStr">
@@ -4345,14 +4353,14 @@
       </c>
       <c r="E127" s="1" t="inlineStr">
         <is>
-          <t>8_relaxed_blanked_3me-12222022142425.avi</t>
+          <t>9_holdbreathing_blanked_2me-12222022141159.avi</t>
         </is>
       </c>
       <c r="F127" t="n">
-        <v>1935</v>
+        <v>3380</v>
       </c>
       <c r="G127" t="n">
-        <v>193.5</v>
+        <v>338</v>
       </c>
       <c r="H127" t="n">
         <v>10</v>
@@ -4374,14 +4382,14 @@
       </c>
       <c r="E128" s="1" t="inlineStr">
         <is>
-          <t>8_relaxed_withoutblanked_3me-12222022141804.avi</t>
+          <t>9_holdbreath_wob2_2me-12222022140630.avi</t>
         </is>
       </c>
       <c r="F128" t="n">
-        <v>3569</v>
+        <v>3570</v>
       </c>
       <c r="G128" t="n">
-        <v>356.9</v>
+        <v>357</v>
       </c>
       <c r="H128" t="n">
         <v>10</v>
@@ -4393,19 +4401,11 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="1" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="B129" s="1" t="inlineStr">
-        <is>
-          <t>2 meters</t>
-        </is>
-      </c>
+      <c r="A129" s="1" t="n"/>
+      <c r="B129" s="1" t="n"/>
       <c r="C129" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>R</t>
         </is>
       </c>
       <c r="D129" s="1" t="inlineStr">
@@ -4415,14 +4415,14 @@
       </c>
       <c r="E129" s="1" t="inlineStr">
         <is>
-          <t>9_holdbreathing_blanked_2me-12222022141159.avi</t>
+          <t>9_relaxedh_blanked2_2me-12222022141019.avi</t>
         </is>
       </c>
       <c r="F129" t="n">
-        <v>3380</v>
+        <v>1654</v>
       </c>
       <c r="G129" t="n">
-        <v>338</v>
+        <v>165.4</v>
       </c>
       <c r="H129" t="n">
         <v>10</v>
@@ -4437,21 +4437,17 @@
       <c r="A130" s="1" t="n"/>
       <c r="B130" s="1" t="n"/>
       <c r="C130" s="1" t="n"/>
-      <c r="D130" s="1" t="inlineStr">
-        <is>
-          <t>WOB</t>
-        </is>
-      </c>
+      <c r="D130" s="1" t="n"/>
       <c r="E130" s="1" t="inlineStr">
         <is>
-          <t>9_holdbreath_wob2_2me-12222022140630.avi</t>
+          <t>9_relaxedh_blanked_2me-12222022140919.avi</t>
         </is>
       </c>
       <c r="F130" t="n">
-        <v>3570</v>
+        <v>1487</v>
       </c>
       <c r="G130" t="n">
-        <v>357</v>
+        <v>148.7</v>
       </c>
       <c r="H130" t="n">
         <v>10</v>
@@ -4465,26 +4461,22 @@
     <row r="131">
       <c r="A131" s="1" t="n"/>
       <c r="B131" s="1" t="n"/>
-      <c r="C131" s="1" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="C131" s="1" t="n"/>
       <c r="D131" s="1" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>WOB</t>
         </is>
       </c>
       <c r="E131" s="1" t="inlineStr">
         <is>
-          <t>9_relaxedh_blanked2_2me-12222022141019.avi</t>
+          <t>9_relaxed_wob2_2me-12222022140457.avi</t>
         </is>
       </c>
       <c r="F131" t="n">
-        <v>1654</v>
+        <v>1546</v>
       </c>
       <c r="G131" t="n">
-        <v>165.4</v>
+        <v>154.6</v>
       </c>
       <c r="H131" t="n">
         <v>10</v>
@@ -4502,14 +4494,14 @@
       <c r="D132" s="1" t="n"/>
       <c r="E132" s="1" t="inlineStr">
         <is>
-          <t>9_relaxedh_blanked_2me-12222022140919.avi</t>
+          <t>9_relaxed_wob_2me-12222022140345.avi</t>
         </is>
       </c>
       <c r="F132" t="n">
-        <v>1487</v>
+        <v>1752</v>
       </c>
       <c r="G132" t="n">
-        <v>148.7</v>
+        <v>175.2</v>
       </c>
       <c r="H132" t="n">
         <v>10</v>
@@ -4522,23 +4514,31 @@
     </row>
     <row r="133">
       <c r="A133" s="1" t="n"/>
-      <c r="B133" s="1" t="n"/>
-      <c r="C133" s="1" t="n"/>
+      <c r="B133" s="1" t="inlineStr">
+        <is>
+          <t>3 meters</t>
+        </is>
+      </c>
+      <c r="C133" s="1" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
       <c r="D133" s="1" t="inlineStr">
         <is>
-          <t>WOB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E133" s="1" t="inlineStr">
         <is>
-          <t>9_relaxed_wob2_2me-12222022140457.avi</t>
+          <t>9_holdbreathing_blanket_3me-12222022143501.avi</t>
         </is>
       </c>
       <c r="F133" t="n">
-        <v>1546</v>
+        <v>1784</v>
       </c>
       <c r="G133" t="n">
-        <v>154.6</v>
+        <v>178.4</v>
       </c>
       <c r="H133" t="n">
         <v>10</v>
@@ -4553,17 +4553,21 @@
       <c r="A134" s="1" t="n"/>
       <c r="B134" s="1" t="n"/>
       <c r="C134" s="1" t="n"/>
-      <c r="D134" s="1" t="n"/>
+      <c r="D134" s="1" t="inlineStr">
+        <is>
+          <t>WOB</t>
+        </is>
+      </c>
       <c r="E134" s="1" t="inlineStr">
         <is>
-          <t>9_relaxed_wob_2me-12222022140345.avi</t>
+          <t>9_holdbreathing_wob_3me-12222022143053.avi</t>
         </is>
       </c>
       <c r="F134" t="n">
-        <v>1752</v>
+        <v>1944</v>
       </c>
       <c r="G134" t="n">
-        <v>175.2</v>
+        <v>194.4</v>
       </c>
       <c r="H134" t="n">
         <v>10</v>
@@ -4576,14 +4580,10 @@
     </row>
     <row r="135">
       <c r="A135" s="1" t="n"/>
-      <c r="B135" s="1" t="inlineStr">
-        <is>
-          <t>3 meters</t>
-        </is>
-      </c>
+      <c r="B135" s="1" t="n"/>
       <c r="C135" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>R</t>
         </is>
       </c>
       <c r="D135" s="1" t="inlineStr">
@@ -4593,14 +4593,14 @@
       </c>
       <c r="E135" s="1" t="inlineStr">
         <is>
-          <t>9_holdbreathing_blanket_3me-12222022143501.avi</t>
+          <t>9_relaxed_blanket_3me-12222022143308.avi</t>
         </is>
       </c>
       <c r="F135" t="n">
-        <v>1784</v>
+        <v>1937</v>
       </c>
       <c r="G135" t="n">
-        <v>178.4</v>
+        <v>193.7</v>
       </c>
       <c r="H135" t="n">
         <v>10</v>
@@ -4622,14 +4622,14 @@
       </c>
       <c r="E136" s="1" t="inlineStr">
         <is>
-          <t>9_holdbreathing_wob_3me-12222022143053.avi</t>
+          <t>9_relaxed_wob_3me-12222022142904.avi</t>
         </is>
       </c>
       <c r="F136" t="n">
-        <v>1944</v>
+        <v>1814</v>
       </c>
       <c r="G136" t="n">
-        <v>194.4</v>
+        <v>181.4</v>
       </c>
       <c r="H136" t="n">
         <v>10</v>
@@ -4640,180 +4640,115 @@
         </is>
       </c>
     </row>
-    <row r="137">
-      <c r="A137" s="1" t="n"/>
-      <c r="B137" s="1" t="n"/>
-      <c r="C137" s="1" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="D137" s="1" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="E137" s="1" t="inlineStr">
-        <is>
-          <t>9_relaxed_blanket_3me-12222022143308.avi</t>
-        </is>
-      </c>
-      <c r="F137" t="n">
-        <v>1937</v>
-      </c>
-      <c r="G137" t="n">
-        <v>193.7</v>
-      </c>
-      <c r="H137" t="n">
-        <v>10</v>
-      </c>
-      <c r="I137" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="1" t="n"/>
-      <c r="B138" s="1" t="n"/>
-      <c r="C138" s="1" t="n"/>
-      <c r="D138" s="1" t="inlineStr">
-        <is>
-          <t>WOB</t>
-        </is>
-      </c>
-      <c r="E138" s="1" t="inlineStr">
-        <is>
-          <t>9_relaxed_wob_3me-12222022142904.avi</t>
-        </is>
-      </c>
-      <c r="F138" t="n">
-        <v>1814</v>
-      </c>
-      <c r="G138" t="n">
-        <v>181.4</v>
-      </c>
-      <c r="H138" t="n">
-        <v>10</v>
-      </c>
-      <c r="I138" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="111">
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="C137:C138"/>
-    <mergeCell ref="A92:A99"/>
+  <mergeCells count="108">
+    <mergeCell ref="A118:A126"/>
+    <mergeCell ref="C39:C41"/>
     <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A127:A136"/>
     <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="B67:B70"/>
     <mergeCell ref="C114:C115"/>
     <mergeCell ref="C71:C72"/>
     <mergeCell ref="C123:C124"/>
-    <mergeCell ref="B116:B119"/>
+    <mergeCell ref="C87:C89"/>
     <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C42:C53"/>
+    <mergeCell ref="D42:D48"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B85:B89"/>
     <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="C44:C55"/>
-    <mergeCell ref="D44:D50"/>
+    <mergeCell ref="D58:D66"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="C73:C75"/>
     <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D60:D68"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="A129:A138"/>
+    <mergeCell ref="C118:C120"/>
+    <mergeCell ref="A80:A89"/>
+    <mergeCell ref="B42:B66"/>
+    <mergeCell ref="B127:B132"/>
     <mergeCell ref="C69:C70"/>
-    <mergeCell ref="B44:B68"/>
-    <mergeCell ref="B73:B77"/>
-    <mergeCell ref="D107:D109"/>
+    <mergeCell ref="D54:D57"/>
     <mergeCell ref="C98:C99"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="C102:C107"/>
+    <mergeCell ref="B90:B93"/>
+    <mergeCell ref="D40:D41"/>
     <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C54:C66"/>
+    <mergeCell ref="B27:B30"/>
     <mergeCell ref="C112:C113"/>
-    <mergeCell ref="B27:B30"/>
     <mergeCell ref="C100:C101"/>
-    <mergeCell ref="C56:C68"/>
-    <mergeCell ref="D51:D55"/>
+    <mergeCell ref="A110:A117"/>
     <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C129:C130"/>
+    <mergeCell ref="C76:C77"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B69:B72"/>
-    <mergeCell ref="B92:B95"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="C131:C134"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="B135:B138"/>
+    <mergeCell ref="C129:C132"/>
+    <mergeCell ref="B133:B136"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="C83:C84"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="A23:A30"/>
-    <mergeCell ref="B125:B128"/>
+    <mergeCell ref="B110:B113"/>
     <mergeCell ref="C116:C117"/>
-    <mergeCell ref="D90:D91"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="A31:A38"/>
-    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="B94:B97"/>
     <mergeCell ref="D131:D132"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="C82:C84"/>
+    <mergeCell ref="A42:A66"/>
+    <mergeCell ref="D80:D81"/>
     <mergeCell ref="A13:A22"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="A44:A68"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="A82:A91"/>
+    <mergeCell ref="B98:B101"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="A98:A109"/>
     <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="D105:D107"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C78:C79"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D133:D134"/>
+    <mergeCell ref="B123:B126"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="A5:A12"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="B129:B134"/>
+    <mergeCell ref="D119:D120"/>
     <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A112:A119"/>
     <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A100:A111"/>
+    <mergeCell ref="B118:B122"/>
     <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C120:C122"/>
-    <mergeCell ref="C104:C109"/>
-    <mergeCell ref="A120:A128"/>
+    <mergeCell ref="C35:C36"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="C133:C134"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="C127:C128"/>
     <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="B80:B84"/>
+    <mergeCell ref="B102:B109"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C135:C136"/>
+    <mergeCell ref="A90:A97"/>
     <mergeCell ref="C110:C111"/>
-    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="A39:A41"/>
     <mergeCell ref="D121:D122"/>
-    <mergeCell ref="B112:B115"/>
-    <mergeCell ref="D104:D106"/>
+    <mergeCell ref="B71:B75"/>
+    <mergeCell ref="D74:D75"/>
     <mergeCell ref="C125:C126"/>
     <mergeCell ref="C96:C97"/>
-    <mergeCell ref="B120:B124"/>
-    <mergeCell ref="D123:D124"/>
+    <mergeCell ref="D129:D130"/>
+    <mergeCell ref="D49:D53"/>
+    <mergeCell ref="A67:A75"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C75:C77"/>
-    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="B114:B117"/>
     <mergeCell ref="C37:C38"/>
-    <mergeCell ref="A69:A77"/>
-    <mergeCell ref="B104:B111"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C80:C82"/>
     <mergeCell ref="C92:C93"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added option extra cells to run for specific file types
</commit_message>
<xml_diff>
--- a/records/xlsx/thermal.xlsx
+++ b/records/xlsx/thermal.xlsx
@@ -1786,16 +1786,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="inlineStr">
-        <is>
-          <t>14_1</t>
-        </is>
-      </c>
-      <c r="B42" s="1" t="inlineStr">
-        <is>
-          <t>2 meters</t>
-        </is>
-      </c>
+      <c r="A42" s="1" t="n"/>
+      <c r="B42" s="1" t="n"/>
       <c r="C42" s="1" t="inlineStr">
         <is>
           <t>R</t>
@@ -1808,21 +1800,21 @@
       </c>
       <c r="E42" s="1" t="inlineStr">
         <is>
-          <t>14_relaxed_wob_2me-12222022162257.avi</t>
+          <t>14_relaxed_blanked_2me-12222022162724.avi</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>2310</v>
+        <v>2255</v>
       </c>
       <c r="G42" t="n">
-        <v>231</v>
+        <v>225.5</v>
       </c>
       <c r="H42" t="n">
         <v>10</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>14_1</t>
+          <t>14</t>
         </is>
       </c>
     </row>
@@ -1837,21 +1829,21 @@
       </c>
       <c r="E43" s="1" t="inlineStr">
         <is>
-          <t>14_relaxed_blanked_2me-12222022162724.avi</t>
+          <t>14_relaxed_wob_2me-12222022162257.avi</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>2255</v>
+        <v>2310</v>
       </c>
       <c r="G43" t="n">
-        <v>225.5</v>
+        <v>231</v>
       </c>
       <c r="H43" t="n">
         <v>10</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>14_1</t>
+          <t>14</t>
         </is>
       </c>
     </row>
@@ -4711,14 +4703,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="111">
+  <mergeCells count="109">
     <mergeCell ref="B82:B86"/>
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="C137:C138"/>
     <mergeCell ref="A92:A99"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="C94:C95"/>
-    <mergeCell ref="B42:B43"/>
     <mergeCell ref="C114:C115"/>
     <mergeCell ref="C71:C72"/>
     <mergeCell ref="C123:C124"/>
@@ -4755,15 +4746,15 @@
     <mergeCell ref="B92:B95"/>
     <mergeCell ref="C102:C103"/>
     <mergeCell ref="C131:C134"/>
-    <mergeCell ref="B39:B41"/>
     <mergeCell ref="C87:C88"/>
     <mergeCell ref="B135:B138"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="A23:A30"/>
     <mergeCell ref="B125:B128"/>
+    <mergeCell ref="B39:B43"/>
     <mergeCell ref="C116:C117"/>
+    <mergeCell ref="C5:C6"/>
     <mergeCell ref="D90:D91"/>
-    <mergeCell ref="C5:C6"/>
     <mergeCell ref="A31:A38"/>
     <mergeCell ref="C73:C74"/>
     <mergeCell ref="D131:D132"/>
@@ -4779,6 +4770,7 @@
     <mergeCell ref="A82:A91"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="C23:C24"/>
+    <mergeCell ref="A39:A43"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C78:C79"/>
     <mergeCell ref="B2:B4"/>
@@ -4805,9 +4797,7 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C135:C136"/>
     <mergeCell ref="C110:C111"/>
-    <mergeCell ref="A39:A41"/>
     <mergeCell ref="D56:D59"/>
-    <mergeCell ref="A42:A43"/>
     <mergeCell ref="D121:D122"/>
     <mergeCell ref="B112:B115"/>
     <mergeCell ref="D104:D106"/>

</xml_diff>